<commit_message>
update new data crawl
</commit_message>
<xml_diff>
--- a/datasets/Crawl-nha_hang_tripadvisor.xlsx
+++ b/datasets/Crawl-nha_hang_tripadvisor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\Hackathon\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1A6AEAC-EB87-448B-8BB5-CB4E0C73B7D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC13B9C4-08BA-44F0-BC1B-5A0A96B6B6C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5745" xr2:uid="{D96E981F-5119-4A7B-8B62-EAA0616E1B03}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$G$315</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$G$304</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="307">
   <si>
     <t>Review</t>
   </si>
@@ -63,21 +63,12 @@
     <t>CocoCamp có view biển nhìn cực đã mắt, lại có đồ ăn ngon, hải sản rẻ. Vừa đc ăn ngon vừa ngắm cảnh bao la đại dương thích ơi là thích ấy. Nếu có cơ hội quay lại Quy Nhơn và Hòn Khô nhất định sẽ ghé nhà hàng CocoCamp</t>
   </si>
   <si>
-    <t>Mình đi gia đình gồm 5 người, view nhà hàng cực đẹp, nhìn ra xa thấy Hòn Khô, nhà mình đăng ký đi tour Hòn Khô Kỳ Co của bên nhà hàng trước đó qua sđt 0905333379 với giá 490k/ người, đồ ăn hải sản tươi sống cực ngon, nhân viên cực nhiệt tình và thân thiện ^^ Chuyến đi thật tuyệt vời, mình sẽ quay lại nơi đây lần nữa.</t>
-  </si>
-  <si>
-    <t>Mình ở ngay Mường Thanh. Cả nhà đói và mệt sau chặng bay từ Hà nội. Đi bộ vài bước mừng như bắt được vàng, nhà chỉ muốn ăn đơn giản nên gọi đĩa rau muống luộc, bát canh cá chua lèo tèo vài miếng vá bớp. Đĩa mực chiên khoảng hai chục miếng. Hai chai nước suối. Lúc đứng dậy hết 379k. Mình chưa nói đến giá, ngoài canh cá còn tạm được. Cơm cũ và nguội. Mực thì chiên quá lửa.... Sao có những người đánh giá tốt được ở nhà hàng này??? Hay tại mình là người Bắc??</t>
-  </si>
-  <si>
     <t>Nằm cuối đường Nguyễn Huệ, khách hàng chủ yếu là dân địa phương. Giá hải sản ở đây rất rẻ so với những nhà hàng ở đường Xuân Diệu. Khách khá đông nên phục vụ không nhanh.</t>
   </si>
   <si>
     <t>Chúng tôi đặt bàn cho 6 người cách đây vài ngày. Chúng tôi đến khoảng 7. 30 giờ tối và có ít hải sản sống. Tuy nhiên người quản lý đã cho chúng tôi 3 con cua đỏ cuối cùng. . . siêu 5 sao cua. Tôi đã đề nghị của anh ta không chọn những con cua xanh lớn hơn và nó không làm chúng tôi thất vọng. Chúng tôi đã nướng tôm và yêu nó. Nhà hàng phục vụ nước sốt cay xanh cay. . . hương vị đặc biệt.</t>
   </si>
   <si>
-    <t>Chúng tôi đã đến thăm quán bar thể thao Quy Nhơn vài lần và rất thích thú. Có một thực đơn tốt với nhiều loại bao gồm cả rau như chúng tôi. Cà ri chay, bánh burger chay &amp; bánh pizza đều ngon - cà ri rất tuyệt. Sạch sẽ và chạy rất tốt - nơi này xứng đáng để làm tốt. Lựa chọn tuyệt vời của các loại bia và khu vực quầy bar / nhà hàng trên tầng 4 là giá trị nỗ lực lên cầu thang. Nếu bạn đang tìm kiếm một break từ mì vv và một chút nấu ăn phương Tây nơi này là lý tưởng, và nó có giá trị một chuyến thăm nếu bạn muốn dính vào thức ăn địa phương là tốt.</t>
-  </si>
-  <si>
     <t>Nhà hàng có khung cảnh rất lãng mạn và ấm cúng. Thức ăn rất nhiều sự lựa chọn, đặc biệt là beef steak có chất lượng ngon nhất trong số những nhà hàng Âu ở Quy Nhơn mà tôi từng trải nghiệm</t>
   </si>
   <si>
@@ -93,15 +84,6 @@
     <t>Nhà hàng Sea Fire Salt mang phong cách châu Âu, món ăn được thiết kế đặc biệt đến bất ngờ, lần đầu tiên tôi được thấy viên đá muối Hymalya được dùng để nướng hải sản và thịt. Điều thua vị về tuổi đời 200 triệu năm, wow, và phải đạt về nhiệt độ phù hợp 200 độ C, theo như lời giới thiệu của bạn Linh nhân viên nhà hàng, tất cả khoáng chất sẽ đi vào bên trong đồ ăn làm cho món ăn đặc biệt hấp dẫn. Sau đó, chiếc xe có hơn 20 loại hương vị muối đã làm cho mn thích thú, tha hồ mà thưởng thức tiệc muối. Cảm ơn bạn Sương và Linh luôn xuất hiện với nụ cười thân thiện. Highly recommend.</t>
   </si>
   <si>
-    <t>Sea Fire Salt là nhà hàng độc đáo nhất mà tôi thấy, với concept đá muối Himalaya tuổi đời 200 năm có nguồn gốc từ Parkistan. Các đầu bếp tài ba đã sử dụng để nướng các loại hải sản và thịt, để nướng được món ăn, viên đá cần được làm nóng và đạt nhiệt độ 200○C. Không thể tin được. Món ăn sẽ thêm vị vì rất nhiều khoáng chất sẽ đi vào trong đồ ăn. Ngoài ra, nhà hàng có 20 loại hương vị muối khác nhau để có thể lựa chọn phù hợp với món ăn. Nhân viên cực kì thân thiện và dễ gần, bạn Sương, Linh và Vy luôn quan tâm và để ý tới gia đình tôi. Cảm ơn nhà hàng đã cho tôi và gia đình những trải nghiệm khó quên. Highly recommend.</t>
-  </si>
-  <si>
-    <t>Nhân viên nhà hàng phục vụ rất nhiệt tình chu đáo đặc biệt bạn Linh, Ân và đồ ăn sáng rất ngon ( bún chả cá và các loại bánh ). Rất thích nơi này nhất định sẽ quay lại lần nữa.</t>
-  </si>
-  <si>
-    <t>Đồ ăn ở đây khá ngon.Nhân viên ở đây như là cô Như phục vụ rất thân thiện.Mặc dù buffet buổi sáng hơi ít đồ ăn nhưng tôi rất thích nhà hàng này.</t>
-  </si>
-  <si>
     <t>Nhà hàng đồ ăn rất ngon , hợp khẩu vị cho gia đình . Không gian thoải mái , mát mẻ rộng rãi .. Sẽ quay lại vào ngày gần nhất</t>
   </si>
   <si>
@@ -120,18 +102,6 @@
     <t>Thấy mọi người đánh giá tốt nên vào ăn thử. Nhưng thực sự là thất vọng và không muốn quay lại quán này luôn. Mình ở phòng Vip, phòng hôi dình, nhân viên phục vụ chậm chạp, đồ ăn không ngon, nguội. Giá thì quá đắt so với nhà hàng Hương Việt ngay bên cạnh mà lại đẳng cấp hơn hẳn. Nói chung là quán này mọi người k nên vào. Cứ vào Hương Việt ăn vừa ngon, sạch sẽ, giá hợp lý, quán lại sang trọng, ngồi phòng Vip giá vẫn giữ nguyên so với bt.. Nói chung là dịch vụ quá tệ so với mức tiền bỏ ra.</t>
   </si>
   <si>
-    <t>Nhà hàng này không xa khách sạn của tôi, không có nhiều người ở đó trên đường 6 giờ chiều, nên tôi ăn tối nhẹ. Đó là tốt, dịch vụ là nhanh chóng.</t>
-  </si>
-  <si>
-    <t>U phải đến đây! Quy Nhơn nói chung thật sự làm chúng tôi ngạc nhiên. Nếu bạn đi đến miền Bắc Việt Nam, họ đang rất bận rộn khi bán đồ cho bạn nhưng ở đây ở Quy nhơn mọi người đều mỉm cười và cố gắng giúp đỡ bạn, điều này là soooo sau 2 tuần liên tục (mua sắm mua sắm). . Dù sao về nhà hàng thực tế.  - Họ không nói tiếng Anh nhưng rất thân thiện (Ban đầu nó có vẻ có vẻ thân thiện nhưng đừng lo lắng họ sẽ không lừa đảo bạn - họ thật sự rất tốt.  - giá khá rẻ (Chúng tôi đã trả 340.000 đồng cho 3 món khai vị, sau đó là 2 món chính (cả hai đều tuyệt vời) - một số món thịt heo và một ít thịt cua). . Bạn phải thử điều này vì họ thực sự đánh giá cao chuyến thăm của bạn và thật tuyệt vời.</t>
-  </si>
-  <si>
-    <t>Thức ăn hoàn toàn tuyệt vời. Không có nhà hàng nào tốt hơn nhà hàng này ở Quy Nhơn. NHÀ HÀNG TỐT NHẤT Ở QUY NHƠN LÀ ĐÂY!</t>
-  </si>
-  <si>
-    <t>Nhóm chúng tôi đến thăm năm ngoái và đến nhà hàng cho bữa ăn đầu tiên trong năm nay. Nó ngon như đã nhớ.</t>
-  </si>
-  <si>
     <t>Món ngon và đặc biệt giá cả hợp lý, nhân viên thì phục vụ chu đáo nhiệt tình. Nhà hàng thì rộng rãi thoáng mát.</t>
   </si>
   <si>
@@ -142,9 +112,6 @@
   </si>
   <si>
     <t>Tôi ở Quy nhơn trong 4 ngày và đã quay lại lần thứ 2 để thưởng thức thêm về các loại bánh đặc sản ở đây: Bánh bột lọc, bánh khoái, bánh cuốn, bánh gio,... và rất nhiều loại bánh tôi không thể nhớ tên dù đã hỏi đến 3 lần, mà bánh nào cũng rất ngon và đẹp. Tôi còn được ăn cả bún tôm. Mỗi món ăn đều được phục vụ nhanh và chăm chút rất đẹp mắt, đầu bếp ở đây chắc hẳn là một người có tâm với nghề. Ngồi tại nhà hàng làm theo mô hình nhà cổ và ăn những món ăn truyền thống được chăm chút cầu kỳ tôi có cảm giác như đây chính là những món ăn của tầng lớp thượng lưu thời xưa. Quán ăn gần đối diện với Tháp đôi Quy nhơn.</t>
-  </si>
-  <si>
-    <t>Quan co cho ngoi ngoai san thoang mat, gia dinh minh co nguoi an kieng va khong thich 1 so gia vi, nha hang phuc vu dung yeu cau. Thuc don da dang va gia ca hop ly, do an trinh bay sach se</t>
   </si>
   <si>
     <t>Các món ăn ở đây rất đa dạng, cách trưng bày thức ăn rất chuyên nghiệp, cứ tưởng như đang đến một nhà hàng 5 sao nào đấy :D. Không gian quán thoát mát, phụ vụ nhiệt tình và cô chủ quán rất dễ thương, tiếp đãi chúng tôi rất ân cần.. Tóm lại, đây là một nhà hàng sẽ nằm trong danh sách các nhà hàng yêu thích của tôi khi trở lại Quy Nhơn thân yêu.</t>
@@ -1067,8 +1034,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{23B176B4-3871-40A7-BE11-CAB9F63EDD0C}" name="data_preprocess_nha_hang_3" displayName="data_preprocess_nha_hang_3" ref="A1:G315" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G315" xr:uid="{1AD48B73-3C38-4C13-B20C-60081022048A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{23B176B4-3871-40A7-BE11-CAB9F63EDD0C}" name="data_preprocess_nha_hang_3" displayName="data_preprocess_nha_hang_3" ref="A1:G304" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G304" xr:uid="{1AD48B73-3C38-4C13-B20C-60081022048A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{35A05C78-451C-44CD-A772-D29BE1720954}" uniqueName="1" name="Review" queryTableFieldId="1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{9A5B63E8-94E5-491E-929B-DA725EF1BD7A}" uniqueName="2" name="giai_tri" queryTableFieldId="2"/>
@@ -1379,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB59D79-8065-43D7-ACAD-CC4A54EAD0D8}">
-  <dimension ref="A1:G315"/>
+  <dimension ref="A1:G304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,16 +1391,16 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1453,7 +1420,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1476,10 +1443,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1499,10 +1466,10 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1522,10 +1489,10 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1545,10 +1512,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1568,10 +1535,10 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1591,10 +1558,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1614,10 +1581,10 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1637,10 +1604,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1660,10 +1627,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1683,10 +1650,10 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1706,10 +1673,10 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1729,10 +1696,10 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1752,10 +1719,10 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1775,10 +1742,10 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1798,10 +1765,10 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1821,10 +1788,10 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1844,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2456,7 +2423,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>306</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -2479,7 +2446,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -2502,7 +2469,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -2525,7 +2492,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -2548,7 +2515,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -2571,7 +2538,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -2594,7 +2561,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -2617,7 +2584,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -2640,7 +2607,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -2663,7 +2630,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -2686,7 +2653,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -2709,7 +2676,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>317</v>
+        <v>62</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -7631,7 +7598,7 @@
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B272">
         <v>0</v>
@@ -7654,7 +7621,7 @@
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B273">
         <v>0</v>
@@ -7677,7 +7644,7 @@
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B274">
         <v>0</v>
@@ -7700,7 +7667,7 @@
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B275">
         <v>0</v>
@@ -7723,7 +7690,7 @@
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B276">
         <v>0</v>
@@ -7746,7 +7713,7 @@
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B277">
         <v>0</v>
@@ -7769,7 +7736,7 @@
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B278">
         <v>0</v>
@@ -7792,7 +7759,7 @@
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B279">
         <v>0</v>
@@ -7815,7 +7782,7 @@
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B280">
         <v>0</v>
@@ -7838,7 +7805,7 @@
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B281">
         <v>0</v>
@@ -7861,7 +7828,7 @@
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B282">
         <v>0</v>
@@ -7884,7 +7851,7 @@
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B283">
         <v>0</v>
@@ -8183,7 +8150,7 @@
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B296">
         <v>0</v>
@@ -8206,7 +8173,7 @@
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B297">
         <v>0</v>
@@ -8229,7 +8196,7 @@
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B298">
         <v>0</v>
@@ -8252,7 +8219,7 @@
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B299">
         <v>0</v>
@@ -8275,7 +8242,7 @@
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B300">
         <v>0</v>
@@ -8298,7 +8265,7 @@
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B301">
         <v>0</v>
@@ -8321,7 +8288,7 @@
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B302">
         <v>0</v>
@@ -8344,7 +8311,7 @@
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B303">
         <v>0</v>
@@ -8367,7 +8334,7 @@
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B304">
         <v>0</v>
@@ -8385,259 +8352,6 @@
         <v>0</v>
       </c>
       <c r="G304">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A305" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B305">
-        <v>0</v>
-      </c>
-      <c r="C305">
-        <v>0</v>
-      </c>
-      <c r="D305">
-        <v>0</v>
-      </c>
-      <c r="E305">
-        <v>0</v>
-      </c>
-      <c r="F305">
-        <v>0</v>
-      </c>
-      <c r="G305">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A306" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B306">
-        <v>0</v>
-      </c>
-      <c r="C306">
-        <v>0</v>
-      </c>
-      <c r="D306">
-        <v>0</v>
-      </c>
-      <c r="E306">
-        <v>0</v>
-      </c>
-      <c r="F306">
-        <v>0</v>
-      </c>
-      <c r="G306">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A307" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B307">
-        <v>0</v>
-      </c>
-      <c r="C307">
-        <v>0</v>
-      </c>
-      <c r="D307">
-        <v>0</v>
-      </c>
-      <c r="E307">
-        <v>0</v>
-      </c>
-      <c r="F307">
-        <v>0</v>
-      </c>
-      <c r="G307">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A308" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B308">
-        <v>0</v>
-      </c>
-      <c r="C308">
-        <v>0</v>
-      </c>
-      <c r="D308">
-        <v>0</v>
-      </c>
-      <c r="E308">
-        <v>0</v>
-      </c>
-      <c r="F308">
-        <v>0</v>
-      </c>
-      <c r="G308">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A309" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B309">
-        <v>0</v>
-      </c>
-      <c r="C309">
-        <v>0</v>
-      </c>
-      <c r="D309">
-        <v>0</v>
-      </c>
-      <c r="E309">
-        <v>0</v>
-      </c>
-      <c r="F309">
-        <v>0</v>
-      </c>
-      <c r="G309">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A310" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B310">
-        <v>0</v>
-      </c>
-      <c r="C310">
-        <v>0</v>
-      </c>
-      <c r="D310">
-        <v>0</v>
-      </c>
-      <c r="E310">
-        <v>0</v>
-      </c>
-      <c r="F310">
-        <v>0</v>
-      </c>
-      <c r="G310">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A311" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B311">
-        <v>0</v>
-      </c>
-      <c r="C311">
-        <v>0</v>
-      </c>
-      <c r="D311">
-        <v>0</v>
-      </c>
-      <c r="E311">
-        <v>0</v>
-      </c>
-      <c r="F311">
-        <v>0</v>
-      </c>
-      <c r="G311">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A312" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B312">
-        <v>0</v>
-      </c>
-      <c r="C312">
-        <v>0</v>
-      </c>
-      <c r="D312">
-        <v>0</v>
-      </c>
-      <c r="E312">
-        <v>0</v>
-      </c>
-      <c r="F312">
-        <v>0</v>
-      </c>
-      <c r="G312">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A313" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B313">
-        <v>0</v>
-      </c>
-      <c r="C313">
-        <v>0</v>
-      </c>
-      <c r="D313">
-        <v>0</v>
-      </c>
-      <c r="E313">
-        <v>0</v>
-      </c>
-      <c r="F313">
-        <v>0</v>
-      </c>
-      <c r="G313">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A314" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B314">
-        <v>0</v>
-      </c>
-      <c r="C314">
-        <v>0</v>
-      </c>
-      <c r="D314">
-        <v>0</v>
-      </c>
-      <c r="E314">
-        <v>0</v>
-      </c>
-      <c r="F314">
-        <v>0</v>
-      </c>
-      <c r="G314">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A315" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="B315">
-        <v>0</v>
-      </c>
-      <c r="C315">
-        <v>0</v>
-      </c>
-      <c r="D315">
-        <v>0</v>
-      </c>
-      <c r="E315">
-        <v>0</v>
-      </c>
-      <c r="F315">
-        <v>0</v>
-      </c>
-      <c r="G315">
         <v>0</v>
       </c>
     </row>

</xml_diff>